<commit_message>
Working on Shader State
</commit_message>
<xml_diff>
--- a/DX_study/DX_study/Data/CSV/MaterialTable.xlsx
+++ b/DX_study/DX_study/Data/CSV/MaterialTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\source\repos\2020_DirectX_Project\DX_study\DX_study\Data\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0690A87B-D986-44B3-B1CC-DACCD0DE33DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2613693D-9771-4B97-A240-DCD933457A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1644" windowWidth="17280" windowHeight="8952" xr2:uid="{F553E549-D7D4-4838-9823-4E194DD1707F}"/>
+    <workbookView xWindow="1404" yWindow="2796" windowWidth="17280" windowHeight="8952" xr2:uid="{F553E549-D7D4-4838-9823-4E194DD1707F}"/>
   </bookViews>
   <sheets>
     <sheet name="MaterialTable" sheetId="1" r:id="rId1"/>
@@ -33,17 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
-  <si>
-    <t>VertexShader</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>PixelShader</t>
-  </si>
-  <si>
     <t>Leather_Normal</t>
   </si>
   <si>
@@ -117,35 +111,10 @@
   </si>
   <si>
     <t>255/255/255/255</t>
-  </si>
-  <si>
-    <t>PerObject</t>
-  </si>
-  <si>
-    <t>Mesh</t>
   </si>
   <si>
     <t>FurTest</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FurMesh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FurShell_ps</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GeometryShader</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FurShell_gs</t>
   </si>
   <si>
     <t>leopard</t>
@@ -269,7 +238,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -283,9 +252,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -606,108 +572,87 @@
   <dimension ref="A1:IU11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11.19921875" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" customWidth="1"/>
-    <col min="6" max="6" width="17.19921875" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="10" max="10" width="15.796875" customWidth="1"/>
-    <col min="14" max="14" width="16.796875" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="11" max="11" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="2">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2">
         <v>1</v>
       </c>
       <c r="O2" s="2"/>
@@ -954,45 +899,36 @@
     </row>
     <row r="3" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="K3" s="2">
         <v>1</v>
       </c>
       <c r="O3" s="2"/>
@@ -1239,45 +1175,36 @@
     </row>
     <row r="4" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="2">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
         <v>1</v>
       </c>
       <c r="O4" s="2"/>
@@ -1524,89 +1451,71 @@
     </row>
     <row r="5" spans="1:255" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="4">
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="O6" s="2"/>
@@ -1853,45 +1762,36 @@
     </row>
     <row r="7" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="O7" s="2"/>
@@ -2138,45 +2038,36 @@
     </row>
     <row r="8" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="K8" s="2">
         <v>1</v>
       </c>
       <c r="O8" s="2"/>
@@ -2423,45 +2314,36 @@
     </row>
     <row r="9" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="K9" s="2">
         <v>1</v>
       </c>
       <c r="O9" s="2"/>
@@ -2708,45 +2590,36 @@
     </row>
     <row r="10" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="2">
-        <v>1</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="K10" s="2">
         <v>1</v>
       </c>
       <c r="O10" s="2"/>
@@ -2993,45 +2866,36 @@
     </row>
     <row r="11" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="2">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="2">
-        <v>1</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="O11" s="2"/>

</xml_diff>

<commit_message>
Update Assimp Texture Loading
</commit_message>
<xml_diff>
--- a/DX_study/DX_study/Data/CSV/MaterialTable.xlsx
+++ b/DX_study/DX_study/Data/CSV/MaterialTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\source\repos\2020_DirectX_Project\DX_study\DX_study\Data\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2613693D-9771-4B97-A240-DCD933457A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B87986-292C-4793-8F8C-C9DE8FF11C3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1404" yWindow="2796" windowWidth="17280" windowHeight="8952" xr2:uid="{F553E549-D7D4-4838-9823-4E194DD1707F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Leather_Albedo</t>
-  </si>
-  <si>
-    <t>Leather_Height</t>
   </si>
   <si>
     <t>RoughnessIntensity</t>
@@ -62,16 +59,10 @@
     <t>AluminiumInsulator</t>
   </si>
   <si>
-    <t>SpecularIntensity</t>
-  </si>
-  <si>
     <t>MetalMap</t>
   </si>
   <si>
     <t>NormalMap</t>
-  </si>
-  <si>
-    <t>SpecularMap</t>
   </si>
   <si>
     <t>AluminiumInsulator_Normal</t>
@@ -81,9 +72,6 @@
   </si>
   <si>
     <t>AluminiumInsulator_Albedo</t>
-  </si>
-  <si>
-    <t>AluminiumInsulator_Height</t>
   </si>
   <si>
     <t>Albedo</t>
@@ -141,6 +129,14 @@
   </si>
   <si>
     <t>PBR_Test5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmissionMap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmissionIntensity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -572,7 +568,7 @@
   <dimension ref="A1:IU11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -583,6 +579,7 @@
     <col min="4" max="4" width="20.3984375" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="10" max="10" width="26.5" customWidth="1"/>
     <col min="11" max="11" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -591,66 +588,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K2" s="2">
         <v>1</v>
@@ -899,28 +896,28 @@
     </row>
     <row r="3" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
@@ -1175,10 +1172,10 @@
     </row>
     <row r="4" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -1190,19 +1187,19 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="I4" s="2">
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>
@@ -1451,34 +1448,34 @@
     </row>
     <row r="5" spans="1:255" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I5" s="4">
         <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K5" s="4">
         <v>1</v>
@@ -1486,28 +1483,28 @@
     </row>
     <row r="6" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
@@ -1762,28 +1759,28 @@
     </row>
     <row r="7" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
@@ -2038,28 +2035,28 @@
     </row>
     <row r="8" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I8" s="2">
         <v>1</v>
@@ -2314,28 +2311,28 @@
     </row>
     <row r="9" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I9" s="2">
         <v>1</v>
@@ -2590,28 +2587,28 @@
     </row>
     <row r="10" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I10" s="2">
         <v>1</v>
@@ -2866,28 +2863,28 @@
     </row>
     <row r="11" spans="1:255" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G11" s="2">
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I11" s="2">
         <v>1</v>

</xml_diff>